<commit_message>
Calculation update regarding last measurements
</commit_message>
<xml_diff>
--- a/DiverMarker/documents/DiverMarker Berechnung Batterielebensdauer.xlsx
+++ b/DiverMarker/documents/DiverMarker Berechnung Batterielebensdauer.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bekone01-my.sharepoint.com/personal/hasan_cetinkaya_beko-technologies_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\_Workspaces\diver_led_tools\DiverMarker\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="8_{A0270BBC-D8E1-451B-B0EB-0B9CE3CA17D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F17F186-9393-46FA-90B7-5F88C9C6B10E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DF6669-1C5B-4594-A76E-44037608B88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C942FD81-DCB5-4068-B906-0A34800DCE0D}"/>
+    <workbookView xWindow="37110" yWindow="-3210" windowWidth="16190" windowHeight="16670" xr2:uid="{C942FD81-DCB5-4068-B906-0A34800DCE0D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="@1 Ohm" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -646,19 +646,19 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="3.7265625" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -667,13 +667,13 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
@@ -685,7 +685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -699,7 +699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -713,7 +713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -724,12 +724,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -743,7 +743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -757,7 +757,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -768,7 +768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -783,7 +783,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -798,7 +798,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -809,13 +809,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="2">
-        <f>50+3</f>
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -824,19 +823,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="4">
         <f>((B12*B13)+(B15*B16))/(1000*3600)</f>
-        <v>1.4722222222222222E-3</v>
+        <v>2.4305555555555556E-3</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -848,25 +847,25 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="4">
         <f>B17+B18</f>
-        <v>3.3888888888888888E-3</v>
+        <v>4.3472222222222219E-3</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="4">
         <f>B19*3600/2.4</f>
-        <v>5.083333333333333</v>
+        <v>6.520833333333333</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
@@ -875,12 +874,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -895,7 +894,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -907,58 +906,58 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="5">
         <f>B5*B20</f>
-        <v>508.33333333333331</v>
+        <v>652.08333333333326</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="5">
         <f>B25+B24</f>
-        <v>724.83333333333326</v>
+        <v>868.58333333333326</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="5">
         <f>B23/B26</f>
-        <v>3.587031501494597</v>
+        <v>2.9933800249448339</v>
       </c>
       <c r="D27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>43</v>
       </c>

</xml_diff>